<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@135f0790f96c372b88922d6bfc9c6d4a49d8140a 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-krebsstadium-cs.xlsx
+++ b/CodeSystem-krebsstadium-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://idg-rlp.de/fhir/tumorkonferenzen/CodeSystem/krebsstadium-cs</t>
+    <t>https://www.uicc.org/resources/tnm</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-22T07:04:28+00:00</t>
+    <t>2024-05-28T11:23:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -108,7 +108,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>5</t>
+    <t>31</t>
   </si>
   <si>
     <t>Level</t>
@@ -126,34 +126,190 @@
     <t>1</t>
   </si>
   <si>
-    <t>stadium0</t>
-  </si>
-  <si>
-    <t>Stadium 0: Tumore ohne Ausbreitung in das Bindegewebe unterhalb der Darmschleimhaut, ohne Lymphknotenbefall und Metastasen</t>
-  </si>
-  <si>
-    <t>stadiumI</t>
-  </si>
-  <si>
-    <t>Stadium I: Kleine und mittelgroße Tumore (T1, T2) ohne Lymphknotenbefall und Metastasen</t>
-  </si>
-  <si>
-    <t>stadiumII</t>
-  </si>
-  <si>
-    <t>Stadium II: Mittelgroße bis große Tumore (T3, T4) ohne Lymphknotenbefall und Metastasen</t>
-  </si>
-  <si>
-    <t>stadiumIII</t>
-  </si>
-  <si>
-    <t>Stadium III: Tumore jeder Größe mit Metastasen in 1-4 Lymphknoten in der Umgebung ohne Fern-Metastasen</t>
-  </si>
-  <si>
-    <t>stadiumIV</t>
-  </si>
-  <si>
-    <t>Stadium IV: Tumore jeder Größe mit Metastasen in 1-4 Lymphknoten in der Umgebung mit Fern-Metastasen</t>
+    <t>okk</t>
+  </si>
+  <si>
+    <t>Stadium X</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Stadium 0</t>
+  </si>
+  <si>
+    <t>0a</t>
+  </si>
+  <si>
+    <t>Stadium 0a</t>
+  </si>
+  <si>
+    <t>0is</t>
+  </si>
+  <si>
+    <t>Stadium 0is</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Stadium I</t>
+  </si>
+  <si>
+    <t>IA1</t>
+  </si>
+  <si>
+    <t>Stadium IA1</t>
+  </si>
+  <si>
+    <t>IA2</t>
+  </si>
+  <si>
+    <t>Stadium IA2</t>
+  </si>
+  <si>
+    <t>IA3</t>
+  </si>
+  <si>
+    <t>Stadium IA3</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>Stadium IB</t>
+  </si>
+  <si>
+    <t>IB1</t>
+  </si>
+  <si>
+    <t>Stadium IB1</t>
+  </si>
+  <si>
+    <t>IB2</t>
+  </si>
+  <si>
+    <t>Stadium IB2</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>Stadium IC</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>Stadium IS</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Stadium II</t>
+  </si>
+  <si>
+    <t>IIA</t>
+  </si>
+  <si>
+    <t>Stadium IIA</t>
+  </si>
+  <si>
+    <t>IIA1</t>
+  </si>
+  <si>
+    <t>Stadium IIA1</t>
+  </si>
+  <si>
+    <t>IIA2</t>
+  </si>
+  <si>
+    <t>Stadium IIA2</t>
+  </si>
+  <si>
+    <t>IIB</t>
+  </si>
+  <si>
+    <t>Stadium IIB</t>
+  </si>
+  <si>
+    <t>IIC</t>
+  </si>
+  <si>
+    <t>Stadium IIC</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>Stadium III</t>
+  </si>
+  <si>
+    <t>IIIA</t>
+  </si>
+  <si>
+    <t>Stadium IIIA</t>
+  </si>
+  <si>
+    <t>IIIA1</t>
+  </si>
+  <si>
+    <t>Stadium IIIA1</t>
+  </si>
+  <si>
+    <t>IIIA2</t>
+  </si>
+  <si>
+    <t>Stadium IIIA2</t>
+  </si>
+  <si>
+    <t>IIIB</t>
+  </si>
+  <si>
+    <t>Stadium IIIB</t>
+  </si>
+  <si>
+    <t>IIIC</t>
+  </si>
+  <si>
+    <t>Stadium IIIC</t>
+  </si>
+  <si>
+    <t>IIIC1</t>
+  </si>
+  <si>
+    <t>Stadium IIIC1</t>
+  </si>
+  <si>
+    <t>IIIC2</t>
+  </si>
+  <si>
+    <t>Stadium IIIC2</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Stadium IV</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>Stadium IVA</t>
+  </si>
+  <si>
+    <t>IVB</t>
+  </si>
+  <si>
+    <t>Stadium IVB</t>
+  </si>
+  <si>
+    <t>IVC</t>
+  </si>
+  <si>
+    <t>Stadium IVC</t>
   </si>
 </sst>
 </file>
@@ -454,7 +610,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -534,6 +690,318 @@
       </c>
       <c r="D6" s="2"/>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>